<commit_message>
Change BAU Dispatch Priority order to put all variable reneable as Priority 1
</commit_message>
<xml_diff>
--- a/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
+++ b/InputData/elec/BDPbES/BAU Dispatch Priority by Elec Source.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\All_states_RMI\CA\elec\BDPbES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\California\Models\eps-california\InputData\elec\BDPbES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{660AF401-9BF3-4F47-8737-4016521A6C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F00613-847E-4EE7-95CD-83EAC14C381F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6910" yWindow="880" windowWidth="18690" windowHeight="11930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -502,9 +502,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -515,32 +515,32 @@
         <v>44463</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -559,16 +559,16 @@
   <dimension ref="A1:AK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
@@ -681,7 +681,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -829,7 +829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -977,7 +977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1569,155 +1569,155 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1865,451 +1865,451 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK12">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2457,155 +2457,155 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <f>$B14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AE14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AG14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK14">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>

</xml_diff>